<commit_message>
Added best and worst cases in ratio analysis
</commit_message>
<xml_diff>
--- a/Ex5/Ex5-RatioAnalysis.xlsx
+++ b/Ex5/Ex5-RatioAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3122225002094\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8945C206-BD92-49A3-876C-214C632BAC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54530141-059E-4863-8F7F-CD691B23A57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AECC5CE0-9EBF-4C29-A032-D41D11570B50}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AECC5CE0-9EBF-4C29-A032-D41D11570B50}"/>
   </bookViews>
   <sheets>
     <sheet name="Bubble Sort" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
   <si>
     <t>Degree(n)</t>
   </si>
@@ -137,6 +137,21 @@
   </si>
   <si>
     <t>Ratio Analysis of Selection Sorting</t>
+  </si>
+  <si>
+    <t>Best Case</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Number of Comparisons</t>
+  </si>
+  <si>
+    <t>Number of Swappings</t>
+  </si>
+  <si>
+    <t>Worst Case</t>
   </si>
 </sst>
 </file>
@@ -202,16 +217,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A6BFE7F-A631-43D8-8490-2204E271E647}">
-  <dimension ref="B2:O11"/>
+  <dimension ref="B2:O21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,22 +566,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -621,7 +637,7 @@
       <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>1.20000913739204E-6</v>
       </c>
       <c r="F4" s="2">
@@ -675,7 +691,7 @@
       <c r="D5" s="2">
         <v>22.4</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>1.12999696284532E-5</v>
       </c>
       <c r="F5" s="2">
@@ -1041,6 +1057,76 @@
       <c r="O11" s="2">
         <f t="shared" si="9"/>
         <v>4.9994999999999998E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1.08999665826559E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1.7500016838312102E-5</v>
       </c>
     </row>
   </sheetData>
@@ -1054,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB26A7D-A02E-4057-A1A1-985F7D02CE78}">
-  <dimension ref="B2:O11"/>
+  <dimension ref="B2:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,22 +1164,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1149,7 +1235,7 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>2.5000190362334201E-6</v>
       </c>
       <c r="F4" s="2">
@@ -1203,7 +1289,7 @@
       <c r="D5" s="2">
         <v>10</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>7.9400371760129905E-6</v>
       </c>
       <c r="F5" s="2">
@@ -1569,6 +1655,76 @@
       <c r="O11" s="2">
         <f t="shared" si="9"/>
         <v>4.9994999999999998E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="5">
+        <v>7.9999445006251301E-6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="5">
+        <v>8.9999521151185002E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added analysis for insertion sort
</commit_message>
<xml_diff>
--- a/Ex5/Ex5-RatioAnalysis.xlsx
+++ b/Ex5/Ex5-RatioAnalysis.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3122225002094\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PyCharmProjects\DSALab\Ex5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54530141-059E-4863-8F7F-CD691B23A57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCAA500-830E-4743-A1C1-170391E5D04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AECC5CE0-9EBF-4C29-A032-D41D11570B50}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{AECC5CE0-9EBF-4C29-A032-D41D11570B50}"/>
   </bookViews>
   <sheets>
     <sheet name="Bubble Sort" sheetId="1" r:id="rId1"/>
     <sheet name="Selection Sort" sheetId="4" r:id="rId2"/>
+    <sheet name="Insertion Sort" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
   <si>
     <t>Degree(n)</t>
   </si>
@@ -153,6 +154,12 @@
   <si>
     <t>Worst Case</t>
   </si>
+  <si>
+    <t>Ratio Analysis of Insertion Sorting</t>
+  </si>
+  <si>
+    <t>Number of overwritings</t>
+  </si>
 </sst>
 </file>
 
@@ -224,10 +231,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,46 +551,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A6BFE7F-A631-43D8-8490-2204E271E647}">
   <dimension ref="B2:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,7 +634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -681,7 +688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>10</v>
       </c>
@@ -735,7 +742,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>50</v>
       </c>
@@ -789,7 +796,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>100</v>
       </c>
@@ -843,7 +850,7 @@
         <v>4.9500000000000004E-3</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>500</v>
       </c>
@@ -897,7 +904,7 @@
         <v>9.9799999999999997E-4</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>1000</v>
       </c>
@@ -951,7 +958,7 @@
         <v>4.9950000000000005E-4</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>5000</v>
       </c>
@@ -1005,7 +1012,7 @@
         <v>9.9980000000000002E-5</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>10000</v>
       </c>
@@ -1059,7 +1066,7 @@
         <v>4.9994999999999998E-5</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -1070,7 +1077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>18</v>
       </c>
@@ -1078,7 +1085,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>19</v>
       </c>
@@ -1086,15 +1093,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>1.08999665826559E-5</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>20</v>
       </c>
@@ -1105,7 +1112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>18</v>
       </c>
@@ -1113,7 +1120,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>19</v>
       </c>
@@ -1121,11 +1128,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <v>1.7500016838312102E-5</v>
       </c>
     </row>
@@ -1146,42 +1153,42 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1225,7 +1232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -1279,7 +1286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>10</v>
       </c>
@@ -1333,7 +1340,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>50</v>
       </c>
@@ -1387,7 +1394,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>100</v>
       </c>
@@ -1441,7 +1448,7 @@
         <v>4.9500000000000004E-3</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>500</v>
       </c>
@@ -1495,7 +1502,7 @@
         <v>9.9799999999999997E-4</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>1000</v>
       </c>
@@ -1549,7 +1556,7 @@
         <v>4.9950000000000005E-4</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>5000</v>
       </c>
@@ -1603,7 +1610,7 @@
         <v>9.9980000000000002E-5</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>10000</v>
       </c>
@@ -1657,7 +1664,7 @@
         <v>4.9994999999999998E-5</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -1668,7 +1675,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>18</v>
       </c>
@@ -1676,7 +1683,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>19</v>
       </c>
@@ -1684,15 +1691,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>7.9999445006251301E-6</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>20</v>
       </c>
@@ -1703,7 +1710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>18</v>
       </c>
@@ -1711,7 +1718,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>19</v>
       </c>
@@ -1719,12 +1726,610 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>8.9999521151185002E-6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:O2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CC71D0-D69A-4316-B4CB-9DD61A3242A3}">
+  <dimension ref="B2:O22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.1600000000000399E-6</v>
+      </c>
+      <c r="F4" s="2">
+        <f>B4</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <f>LOG10(F4)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <f>F4*G4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <f>POWER(F4,2)</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <f>POWER(F4, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <f>C4/F4</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="2" t="e">
+        <f>C4/G4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M4" s="2" t="e">
+        <f>C4/H4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N4" s="2">
+        <f>C4/I4</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <f>C4/J4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="D5" s="2">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <v>4.31999999999932E-6</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" ref="F5:F11" si="0">B5</f>
+        <v>10</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G11" si="1">LOG10(F5)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" ref="H5:H11" si="2">F5*G5</f>
+        <v>10</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" ref="I5:I11" si="3">POWER(F5,2)</f>
+        <v>100</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" ref="J5:J11" si="4">POWER(F5, 3)</f>
+        <v>1000</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" ref="K5:K11" si="5">C5/F5</f>
+        <v>1.94</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" ref="L5:L11" si="6">C5/G5</f>
+        <v>19.399999999999999</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" ref="M5:M11" si="7">C5/H5</f>
+        <v>1.94</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" ref="N5:N11" si="8">C5/I5</f>
+        <v>0.19399999999999998</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" ref="O5:O11" si="9">C5/J5</f>
+        <v>1.9399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2">
+        <v>663</v>
+      </c>
+      <c r="D6" s="2">
+        <v>663</v>
+      </c>
+      <c r="E6" s="3">
+        <v>8.7160000000002696E-5</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6989700043360187</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="2"/>
+        <v>84.948500216800937</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="3"/>
+        <v>2500</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="4"/>
+        <v>125000</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="5"/>
+        <v>13.26</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="6"/>
+        <v>390.23643637493745</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="7"/>
+        <v>7.8047287274987491</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="8"/>
+        <v>0.26519999999999999</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="9"/>
+        <v>5.3039999999999997E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>100</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2543</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2543</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2.6323999999999499E-4</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="3"/>
+        <v>10000</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="5"/>
+        <v>25.43</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="6"/>
+        <v>1271.5</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="7"/>
+        <v>12.715</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="8"/>
+        <v>0.25430000000000003</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="9"/>
+        <v>2.5430000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>500</v>
+      </c>
+      <c r="C8" s="2">
+        <v>62857.599999999999</v>
+      </c>
+      <c r="D8" s="2">
+        <v>62857.599999999999</v>
+      </c>
+      <c r="E8" s="2">
+        <v>6.1542999999999997E-3</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>2.6989700043360187</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="2"/>
+        <v>1349.4850021680095</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="3"/>
+        <v>250000</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="4"/>
+        <v>125000000</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="5"/>
+        <v>125.7152</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="6"/>
+        <v>23289.477059402805</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="7"/>
+        <v>46.578954118805605</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="8"/>
+        <v>0.2514304</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="9"/>
+        <v>5.0286079999999999E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="2">
+        <v>252100.2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>252100.2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2.6573079999999999E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="2"/>
+        <v>3000</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="3"/>
+        <v>1000000</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000000</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="5"/>
+        <v>252.1002</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="6"/>
+        <v>84033.400000000009</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="7"/>
+        <v>84.0334</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="8"/>
+        <v>0.2521002</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="9"/>
+        <v>2.5210020000000002E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <v>5000</v>
+      </c>
+      <c r="C10" s="2">
+        <v>6222192.4000000004</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6222192.4000000004</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.65331218000000002</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>3.6989700043360187</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="2"/>
+        <v>18494.850021680093</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="3"/>
+        <v>25000000</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="4"/>
+        <v>125000000000</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="5"/>
+        <v>1244.43848</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="6"/>
+        <v>1682141.8915823058</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="7"/>
+        <v>336.42837831646119</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="8"/>
+        <v>0.24888769600000002</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="9"/>
+        <v>4.9777539200000006E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C11" s="2">
+        <v>25013194.800000001</v>
+      </c>
+      <c r="D11" s="2">
+        <v>25013194.800000001</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2.6780067599999899</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="2"/>
+        <v>40000</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="3"/>
+        <v>100000000</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000000000</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="5"/>
+        <v>2501.3194800000001</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="6"/>
+        <v>6253298.7000000002</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="7"/>
+        <v>625.32987000000003</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="8"/>
+        <v>0.25013194799999999</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="9"/>
+        <v>2.5013194799999999E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2.99999999953115E-6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="4">
+        <v>5.6999999991091903E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added documentation for ex 5 and added borders in the Excel file and aligned it properly.
</commit_message>
<xml_diff>
--- a/Ex5/Ex5-RatioAnalysis.xlsx
+++ b/Ex5/Ex5-RatioAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PyCharmProjects\DSALab\Ex5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCAA500-830E-4743-A1C1-170391E5D04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE83FDD-55E3-4DC6-96A5-31DB07742E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{AECC5CE0-9EBF-4C29-A032-D41D11570B50}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{AECC5CE0-9EBF-4C29-A032-D41D11570B50}"/>
   </bookViews>
   <sheets>
     <sheet name="Bubble Sort" sheetId="1" r:id="rId1"/>
@@ -224,16 +224,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -551,56 +559,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A6BFE7F-A631-43D8-8490-2204E271E647}">
   <dimension ref="B2:O21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
     <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" customWidth="1"/>
     <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.77734375" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-    </row>
-    <row r="3" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="2:15" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -624,7 +633,7 @@
       <c r="L3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -1067,72 +1076,72 @@
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>1.08999665826559E-5</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>45</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>1.7500016838312102E-5</v>
       </c>
     </row>
@@ -1149,56 +1158,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB26A7D-A02E-4057-A1A1-985F7D02CE78}">
   <dimension ref="B2:O22"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" customWidth="1"/>
     <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-    </row>
-    <row r="3" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="2:15" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1222,7 +1232,7 @@
       <c r="L3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -1665,72 +1675,72 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>45</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>7.9999445006251301E-6</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>45</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>8.9999521151185002E-6</v>
       </c>
     </row>
@@ -1747,56 +1757,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CC71D0-D69A-4316-B4CB-9DD61A3242A3}">
   <dimension ref="B2:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="2" max="2" width="13" style="5" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" style="5" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" style="5" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-    </row>
-    <row r="3" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+    </row>
+    <row r="3" spans="2:15" ht="63" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1820,7 +1833,7 @@
       <c r="L3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -1831,504 +1844,504 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
+      <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
         <v>1.1600000000000399E-6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="7">
         <f>B4</f>
         <v>1</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="7">
         <f>LOG10(F4)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="7">
         <f>F4*G4</f>
         <v>0</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="7">
         <f>POWER(F4,2)</f>
         <v>1</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="7">
         <f>POWER(F4, 3)</f>
         <v>1</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="7">
         <f>C4/F4</f>
         <v>0</v>
       </c>
-      <c r="L4" s="2" t="e">
+      <c r="L4" s="7" t="e">
         <f>C4/G4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M4" s="2" t="e">
+      <c r="M4" s="7" t="e">
         <f>C4/H4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="7">
         <f>C4/I4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="7">
         <f>C4/J4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
+      <c r="B5" s="7">
         <v>10</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="7">
         <v>19.399999999999999</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="7">
         <v>19.399999999999999</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="8">
         <v>4.31999999999932E-6</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="7">
         <f t="shared" ref="F5:F11" si="0">B5</f>
         <v>10</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="7">
         <f t="shared" ref="G5:G11" si="1">LOG10(F5)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="7">
         <f t="shared" ref="H5:H11" si="2">F5*G5</f>
         <v>10</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="7">
         <f t="shared" ref="I5:I11" si="3">POWER(F5,2)</f>
         <v>100</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="7">
         <f t="shared" ref="J5:J11" si="4">POWER(F5, 3)</f>
         <v>1000</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="7">
         <f t="shared" ref="K5:K11" si="5">C5/F5</f>
         <v>1.94</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="7">
         <f t="shared" ref="L5:L11" si="6">C5/G5</f>
         <v>19.399999999999999</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="7">
         <f t="shared" ref="M5:M11" si="7">C5/H5</f>
         <v>1.94</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="7">
         <f t="shared" ref="N5:N11" si="8">C5/I5</f>
         <v>0.19399999999999998</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="7">
         <f t="shared" ref="O5:O11" si="9">C5/J5</f>
         <v>1.9399999999999997E-2</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
+      <c r="B6" s="7">
         <v>50</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="7">
         <v>663</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="7">
         <v>663</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="8">
         <v>8.7160000000002696E-5</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="7">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="7">
         <f t="shared" si="1"/>
         <v>1.6989700043360187</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="7">
         <f t="shared" si="2"/>
         <v>84.948500216800937</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="7">
         <f t="shared" si="3"/>
         <v>2500</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="7">
         <f t="shared" si="4"/>
         <v>125000</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="7">
         <f t="shared" si="5"/>
         <v>13.26</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="7">
         <f t="shared" si="6"/>
         <v>390.23643637493745</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="7">
         <f t="shared" si="7"/>
         <v>7.8047287274987491</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="7">
         <f t="shared" si="8"/>
         <v>0.26519999999999999</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="7">
         <f t="shared" si="9"/>
         <v>5.3039999999999997E-3</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
+      <c r="B7" s="7">
         <v>100</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="7">
         <v>2543</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="7">
         <v>2543</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="7">
         <v>2.6323999999999499E-4</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="7">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="7">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="7">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="7">
         <f t="shared" si="3"/>
         <v>10000</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="7">
         <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="7">
         <f t="shared" si="5"/>
         <v>25.43</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="7">
         <f t="shared" si="6"/>
         <v>1271.5</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="7">
         <f t="shared" si="7"/>
         <v>12.715</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="7">
         <f t="shared" si="8"/>
         <v>0.25430000000000003</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="7">
         <f t="shared" si="9"/>
         <v>2.5430000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="2">
+      <c r="B8" s="7">
         <v>500</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="7">
         <v>62857.599999999999</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="7">
         <v>62857.599999999999</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="7">
         <v>6.1542999999999997E-3</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="7">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="7">
         <f t="shared" si="1"/>
         <v>2.6989700043360187</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="7">
         <f t="shared" si="2"/>
         <v>1349.4850021680095</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="7">
         <f t="shared" si="3"/>
         <v>250000</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="7">
         <f t="shared" si="4"/>
         <v>125000000</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="7">
         <f t="shared" si="5"/>
         <v>125.7152</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="7">
         <f t="shared" si="6"/>
         <v>23289.477059402805</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="7">
         <f t="shared" si="7"/>
         <v>46.578954118805605</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="7">
         <f t="shared" si="8"/>
         <v>0.2514304</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="7">
         <f t="shared" si="9"/>
         <v>5.0286079999999999E-4</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
+      <c r="B9" s="7">
         <v>1000</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="7">
         <v>252100.2</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="7">
         <v>252100.2</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="7">
         <v>2.6573079999999999E-2</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="7">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="7">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="7">
         <f t="shared" si="2"/>
         <v>3000</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="7">
         <f t="shared" si="3"/>
         <v>1000000</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="7">
         <f t="shared" si="4"/>
         <v>1000000000</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="7">
         <f t="shared" si="5"/>
         <v>252.1002</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="7">
         <f t="shared" si="6"/>
         <v>84033.400000000009</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="7">
         <f t="shared" si="7"/>
         <v>84.0334</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="7">
         <f t="shared" si="8"/>
         <v>0.2521002</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="7">
         <f t="shared" si="9"/>
         <v>2.5210020000000002E-4</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
+      <c r="B10" s="7">
         <v>5000</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="7">
         <v>6222192.4000000004</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="7">
         <v>6222192.4000000004</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="7">
         <v>0.65331218000000002</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="7">
         <f t="shared" si="0"/>
         <v>5000</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="7">
         <f t="shared" si="1"/>
         <v>3.6989700043360187</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="7">
         <f t="shared" si="2"/>
         <v>18494.850021680093</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="7">
         <f t="shared" si="3"/>
         <v>25000000</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="7">
         <f t="shared" si="4"/>
         <v>125000000000</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="7">
         <f t="shared" si="5"/>
         <v>1244.43848</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="7">
         <f t="shared" si="6"/>
         <v>1682141.8915823058</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="7">
         <f t="shared" si="7"/>
         <v>336.42837831646119</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="7">
         <f t="shared" si="8"/>
         <v>0.24888769600000002</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10" s="7">
         <f t="shared" si="9"/>
         <v>4.9777539200000006E-5</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
+      <c r="B11" s="7">
         <v>10000</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="7">
         <v>25013194.800000001</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="7">
         <v>25013194.800000001</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="7">
         <v>2.6780067599999899</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="7">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="7">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="7">
         <f t="shared" si="2"/>
         <v>40000</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="7">
         <f t="shared" si="3"/>
         <v>100000000</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="7">
         <f t="shared" si="4"/>
         <v>1000000000000</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="7">
         <f t="shared" si="5"/>
         <v>2501.3194800000001</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="7">
         <f t="shared" si="6"/>
         <v>6253298.7000000002</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="7">
         <f t="shared" si="7"/>
         <v>625.32987000000003</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="7">
         <f t="shared" si="8"/>
         <v>0.25013194799999999</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="7">
         <f t="shared" si="9"/>
         <v>2.5013194799999999E-5</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
+      <c r="C15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
+      <c r="C17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="8">
         <v>2.99999999953115E-6</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+      <c r="C20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="7">
         <v>45</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
+      <c r="C21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="7">
         <v>45</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
+      <c r="C22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="8">
         <v>5.6999999991091903E-6</v>
       </c>
     </row>

</xml_diff>